<commit_message>
Final Exam problems 1-2
Park and Bank problems
</commit_message>
<xml_diff>
--- a/Unit 9 Integer Optimization/Gerrymandering.xlsx
+++ b/Unit 9 Integer Optimization/Gerrymandering.xlsx
@@ -8,91 +8,181 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcampbell/Documents/GitHub/MIT-Analytics/Unit 9 Integer Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA64955-8486-9944-945F-EF7B2D949890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A891BB-508F-1B4A-A982-52A39C30748C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13800" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$C$5:$E$37</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet2!$C$5:$E$37</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet3!$C$5:$E$37</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Sheet4!$C$5:$E$37</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$C$38:$E$38</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet2!$C$38:$E$38</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Sheet3!$C$38:$E$38</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Sheet4!$C$38:$E$38</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$C$44:$C$45</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet2!$C$44:$C$46</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Sheet3!$C$44:$C$46</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Sheet4!$C$44:$C$52</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$C$5:$E$37</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet2!$C$5:$E$37</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Sheet3!$C$5:$E$37</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Sheet4!$C$5:$E$37</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$I$5:$I$37</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sheet2!$I$5:$I$37</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">Sheet3!$E$47</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Sheet4!$E$57</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">Sheet3!$E$48</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Sheet4!$E$58</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">Sheet3!$I$5:$I$37</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">Sheet4!$I$5:$I$37</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">6</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$C$41</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet2!$C$41</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sheet3!$C$41</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Sheet4!$C$41</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">12000</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">binary</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">binary</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">binary</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">binary</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">Sheet3!$G$47</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">Sheet4!$G$57</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">Sheet3!$G$48</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">Sheet4!$G$58</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -113,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="66">
   <si>
     <t>Gerrymandering New Mexico</t>
   </si>
@@ -275,13 +365,49 @@
   </si>
   <si>
     <t>D2 margin</t>
+  </si>
+  <si>
+    <t>Santa Fe or Dona Ana in D2</t>
+  </si>
+  <si>
+    <t>Socorro and Torrance in same</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>D1 Scenario 1 margin</t>
+  </si>
+  <si>
+    <t>D2 Scenario 1 margin</t>
+  </si>
+  <si>
+    <t>D3 Scenario 1 margin</t>
+  </si>
+  <si>
+    <t>D1 Scenario 2 margin</t>
+  </si>
+  <si>
+    <t>D2 Scenario 2 margin</t>
+  </si>
+  <si>
+    <t>D3 Scenario 2 margin</t>
+  </si>
+  <si>
+    <t>D1 Scenario 3 margin</t>
+  </si>
+  <si>
+    <t>D2 Scenario 3 margin</t>
+  </si>
+  <si>
+    <t>D3 Scenario 3 margin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +454,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -517,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -575,6 +708,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -584,9 +720,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -968,16 +1128,16 @@
     <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="21" t="s">
+      <c r="C3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
@@ -1976,13 +2136,13 @@
       <c r="B37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="24">
-        <v>0</v>
-      </c>
-      <c r="D37" s="24">
-        <v>1</v>
-      </c>
-      <c r="E37" s="25">
+      <c r="C37" s="21">
+        <v>0</v>
+      </c>
+      <c r="D37" s="21">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22">
         <v>0</v>
       </c>
       <c r="F37" s="13">
@@ -2107,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E8546F-71C7-B445-9FA6-628F48330D9F}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2122,7 +2282,7 @@
     <col min="8" max="8" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2135,7 +2295,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2146,22 +2306,22 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="21" t="s">
+      <c r="C3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2190,7 +2350,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -2198,10 +2358,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2219,8 +2379,13 @@
         <f>SUM(C5:E5)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K5" s="27">
+        <v>1</v>
+      </c>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -2228,10 +2393,10 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2249,8 +2414,13 @@
         <f t="shared" ref="I6:I37" si="0">SUM(C6:E6)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K6" s="30"/>
+      <c r="L6" s="31">
+        <v>1</v>
+      </c>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -2261,10 +2431,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="9">
         <v>-6650</v>
@@ -2279,8 +2449,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K7" s="30"/>
+      <c r="L7" s="31">
+        <v>1</v>
+      </c>
+      <c r="M7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -2309,8 +2484,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K8" s="30"/>
+      <c r="L8" s="31">
+        <v>1</v>
+      </c>
+      <c r="M8" s="32"/>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>5</v>
       </c>
@@ -2321,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="9">
         <v>116</v>
@@ -2339,8 +2519,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K9" s="30"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -2369,8 +2554,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -2381,10 +2571,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="9">
         <v>-299</v>
@@ -2399,8 +2589,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K11" s="30"/>
+      <c r="L11" s="31">
+        <v>1</v>
+      </c>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -2411,10 +2606,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="9">
         <v>9790</v>
@@ -2429,8 +2624,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K12" s="30"/>
+      <c r="L12" s="31">
+        <v>1</v>
+      </c>
+      <c r="M12" s="32"/>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>9</v>
       </c>
@@ -2441,10 +2641,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="9">
         <v>-6436</v>
@@ -2459,8 +2659,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K13" s="30"/>
+      <c r="L13" s="31">
+        <v>1</v>
+      </c>
+      <c r="M13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -2489,8 +2694,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K14" s="30"/>
+      <c r="L14" s="31">
+        <v>1</v>
+      </c>
+      <c r="M14" s="32"/>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -2519,8 +2729,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K15" s="30"/>
+      <c r="L15" s="31">
+        <v>1</v>
+      </c>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -2549,8 +2764,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K16" s="30"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -2579,8 +2799,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K17" s="30"/>
+      <c r="L17" s="31">
+        <v>1</v>
+      </c>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -2591,10 +2816,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="9">
         <v>-8412</v>
@@ -2609,8 +2834,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K18" s="30"/>
+      <c r="L18" s="31">
+        <v>1</v>
+      </c>
+      <c r="M18" s="32"/>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>15</v>
       </c>
@@ -2621,10 +2851,10 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="9">
         <v>-3009</v>
@@ -2639,8 +2869,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K19" s="30"/>
+      <c r="L19" s="31">
+        <v>1</v>
+      </c>
+      <c r="M19" s="32"/>
+    </row>
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>16</v>
       </c>
@@ -2651,10 +2886,10 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="9">
         <v>395</v>
@@ -2669,8 +2904,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>17</v>
       </c>
@@ -2681,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="9">
         <v>-81</v>
@@ -2699,8 +2939,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K21" s="30"/>
+      <c r="L21" s="31">
+        <v>1</v>
+      </c>
+      <c r="M21" s="32"/>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>18</v>
       </c>
@@ -2711,10 +2956,10 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="9">
         <v>9943</v>
@@ -2729,8 +2974,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K22" s="30"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>19</v>
       </c>
@@ -2759,8 +3009,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K23" s="30"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>20</v>
       </c>
@@ -2771,10 +3026,10 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="9">
         <v>-5504</v>
@@ -2789,8 +3044,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K24" s="30"/>
+      <c r="L24" s="31">
+        <v>1</v>
+      </c>
+      <c r="M24" s="32"/>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>21</v>
       </c>
@@ -2819,8 +3079,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K25" s="30"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>22</v>
       </c>
@@ -2831,10 +3096,10 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="9">
         <v>8016</v>
@@ -2849,8 +3114,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K26" s="30"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>23</v>
       </c>
@@ -2861,10 +3131,10 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="9">
         <v>-2313</v>
@@ -2879,8 +3149,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K27" s="30"/>
+      <c r="L27" s="31">
+        <v>1</v>
+      </c>
+      <c r="M27" s="32"/>
+    </row>
+    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>24</v>
       </c>
@@ -2891,10 +3166,10 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="9">
         <v>2707</v>
@@ -2909,8 +3184,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K28" s="30"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>25</v>
       </c>
@@ -2939,8 +3219,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K29" s="30"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>26</v>
       </c>
@@ -2951,10 +3236,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="9">
         <v>6473</v>
@@ -2969,8 +3254,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K30" s="30"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>27</v>
       </c>
@@ -2999,8 +3289,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K31" s="30"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>28</v>
       </c>
@@ -3011,10 +3306,10 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="9">
         <v>-965</v>
@@ -3029,8 +3324,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K32" s="30"/>
+      <c r="L32" s="31">
+        <v>1</v>
+      </c>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>29</v>
       </c>
@@ -3038,10 +3338,10 @@
         <v>39</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -3059,8 +3359,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K33" s="30"/>
+      <c r="L33" s="31">
+        <v>1</v>
+      </c>
+      <c r="M33" s="32"/>
+    </row>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>30</v>
       </c>
@@ -3089,8 +3394,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K34" s="30"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>31</v>
       </c>
@@ -3098,13 +3408,13 @@
         <v>41</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="9">
         <v>-1107</v>
@@ -3119,8 +3429,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K35" s="30">
+        <v>1</v>
+      </c>
+      <c r="L35" s="31"/>
+      <c r="M35" s="32"/>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>32</v>
       </c>
@@ -3149,21 +3464,26 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="30"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>33</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="24">
-        <v>0</v>
-      </c>
-      <c r="D37" s="24">
-        <v>1</v>
-      </c>
-      <c r="E37" s="25">
+      <c r="C37" s="21">
+        <v>0</v>
+      </c>
+      <c r="D37" s="21">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22">
         <v>0</v>
       </c>
       <c r="F37" s="13">
@@ -3179,8 +3499,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="K37" s="33"/>
+      <c r="L37" s="34">
+        <v>1</v>
+      </c>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" spans="1:13" ht="28" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="20" t="s">
         <v>52</v>
@@ -3191,18 +3516,18 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" ref="D38:E38" si="1">SUM(D5:D37)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3213,7 +3538,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" t="s">
         <v>44</v>
@@ -3228,24 +3553,24 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C41">
-        <f>SUMPRODUCT(C5:E37,Sheet1!C5:E37)</f>
+        <f>SUMPRODUCT(C5:E37,K5:M37)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C44">
         <f>SUMPRODUCT(C5:C37,F5:F37)</f>
-        <v>368</v>
+        <v>41834</v>
       </c>
       <c r="D44" t="s">
         <v>48</v>
@@ -3254,13 +3579,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B45" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="26">
+      <c r="C45" s="23">
         <f>SUMPRODUCT(F5:F37,D5:D37)</f>
-        <v>110432</v>
+        <v>16330</v>
       </c>
       <c r="D45" t="s">
         <v>48</v>
@@ -3269,19 +3594,2889 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C46">
         <f>SUMPRODUCT(E5:E37,F5:F37)</f>
-        <v>-34403</v>
+        <v>18233</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
       </c>
       <c r="E46" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487F3141-D2D1-0044-A1CA-44EB422BB913}">
+  <dimension ref="A1:M48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>42941</v>
+      </c>
+      <c r="G5" s="7">
+        <v>43411</v>
+      </c>
+      <c r="H5" s="8">
+        <v>11336</v>
+      </c>
+      <c r="I5" s="1">
+        <f>SUM(C5:E5)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="27">
+        <v>1</v>
+      </c>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-917</v>
+      </c>
+      <c r="G6" s="11">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12">
+        <v>-716</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I37" si="0">SUM(C6:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="30"/>
+      <c r="L6" s="31">
+        <v>1</v>
+      </c>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>-6650</v>
+      </c>
+      <c r="G7" s="11">
+        <v>-6244</v>
+      </c>
+      <c r="H7" s="12">
+        <v>-6436</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31">
+        <v>1</v>
+      </c>
+      <c r="M7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>4</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1941</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1449</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1025</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="30"/>
+      <c r="L8" s="31">
+        <v>1</v>
+      </c>
+      <c r="M8" s="32"/>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>116</v>
+      </c>
+      <c r="G9" s="11">
+        <v>-871</v>
+      </c>
+      <c r="H9" s="12">
+        <v>-1099</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="30"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>-5194</v>
+      </c>
+      <c r="G10" s="11">
+        <v>-4241</v>
+      </c>
+      <c r="H10" s="12">
+        <v>-5093</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>-299</v>
+      </c>
+      <c r="G11" s="11">
+        <v>223</v>
+      </c>
+      <c r="H11" s="12">
+        <v>567</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31">
+        <v>1</v>
+      </c>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>9790</v>
+      </c>
+      <c r="G12" s="11">
+        <v>8856</v>
+      </c>
+      <c r="H12" s="12">
+        <v>8251</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31">
+        <v>1</v>
+      </c>
+      <c r="M12" s="32"/>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>-6436</v>
+      </c>
+      <c r="G13" s="11">
+        <v>-6787</v>
+      </c>
+      <c r="H13" s="12">
+        <v>-6736</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="30"/>
+      <c r="L13" s="31">
+        <v>1</v>
+      </c>
+      <c r="M13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1723</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1993</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1121</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="30"/>
+      <c r="L14" s="31">
+        <v>1</v>
+      </c>
+      <c r="M14" s="32"/>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>870</v>
+      </c>
+      <c r="G15" s="11">
+        <v>260</v>
+      </c>
+      <c r="H15" s="12">
+        <v>183</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31">
+        <v>1</v>
+      </c>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>12</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>-66</v>
+      </c>
+      <c r="G16" s="11">
+        <v>-349</v>
+      </c>
+      <c r="H16" s="12">
+        <v>-286</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>13</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9">
+        <v>99</v>
+      </c>
+      <c r="G17" s="11">
+        <v>510</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1014</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="30"/>
+      <c r="L17" s="31">
+        <v>1</v>
+      </c>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>14</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>-8412</v>
+      </c>
+      <c r="G18" s="11">
+        <v>-7585</v>
+      </c>
+      <c r="H18" s="12">
+        <v>-8062</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="30"/>
+      <c r="L18" s="31">
+        <v>1</v>
+      </c>
+      <c r="M18" s="32"/>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>15</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>-3009</v>
+      </c>
+      <c r="G19" s="11">
+        <v>-2233</v>
+      </c>
+      <c r="H19" s="12">
+        <v>-1678</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K19" s="30"/>
+      <c r="L19" s="31">
+        <v>1</v>
+      </c>
+      <c r="M19" s="32"/>
+    </row>
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>395</v>
+      </c>
+      <c r="G20" s="11">
+        <v>-347</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1984</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>17</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>-81</v>
+      </c>
+      <c r="G21" s="11">
+        <v>233</v>
+      </c>
+      <c r="H21" s="12">
+        <v>-371</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="30"/>
+      <c r="L21" s="31">
+        <v>1</v>
+      </c>
+      <c r="M21" s="32"/>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>18</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>9943</v>
+      </c>
+      <c r="G22" s="11">
+        <v>9995</v>
+      </c>
+      <c r="H22" s="12">
+        <v>9711</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="30"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>19</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1361</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1780</v>
+      </c>
+      <c r="H23" s="12">
+        <v>975</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="30"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>20</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>-5504</v>
+      </c>
+      <c r="G24" s="11">
+        <v>-5578</v>
+      </c>
+      <c r="H24" s="12">
+        <v>-5135</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="30"/>
+      <c r="L24" s="31">
+        <v>1</v>
+      </c>
+      <c r="M24" s="32"/>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>21</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>-812</v>
+      </c>
+      <c r="G25" s="11">
+        <v>-992</v>
+      </c>
+      <c r="H25" s="12">
+        <v>-942</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="30"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>22</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9">
+        <v>8016</v>
+      </c>
+      <c r="G26" s="11">
+        <v>7948</v>
+      </c>
+      <c r="H26" s="12">
+        <v>44329</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K26" s="30"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>23</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>-2313</v>
+      </c>
+      <c r="G27" s="11">
+        <v>-2665</v>
+      </c>
+      <c r="H27" s="12">
+        <v>-2263</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K27" s="30"/>
+      <c r="L27" s="31">
+        <v>1</v>
+      </c>
+      <c r="M27" s="32"/>
+    </row>
+    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>24</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>2707</v>
+      </c>
+      <c r="G28" s="11">
+        <v>1984</v>
+      </c>
+      <c r="H28" s="12">
+        <v>5668</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>25</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>-13091</v>
+      </c>
+      <c r="G29" s="11">
+        <v>-13942</v>
+      </c>
+      <c r="H29" s="12">
+        <v>-13488</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="30"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>26</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9">
+        <v>6473</v>
+      </c>
+      <c r="G30" s="11">
+        <v>7008</v>
+      </c>
+      <c r="H30" s="12">
+        <v>7571</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="30"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>27</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9">
+        <v>34523</v>
+      </c>
+      <c r="G31" s="11">
+        <v>34516</v>
+      </c>
+      <c r="H31" s="12">
+        <v>12145</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="30"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>28</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9">
+        <v>-965</v>
+      </c>
+      <c r="G32" s="11">
+        <v>-658</v>
+      </c>
+      <c r="H32" s="12">
+        <v>-173</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="30"/>
+      <c r="L32" s="31">
+        <v>1</v>
+      </c>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>29</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1285</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1491</v>
+      </c>
+      <c r="H33" s="12">
+        <v>3004</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K33" s="30"/>
+      <c r="L33" s="31">
+        <v>1</v>
+      </c>
+      <c r="M33" s="32"/>
+    </row>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>30</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="9">
+        <v>9145</v>
+      </c>
+      <c r="G34" s="11">
+        <v>9779</v>
+      </c>
+      <c r="H34" s="12">
+        <v>10226</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K34" s="30"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>31</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>-1107</v>
+      </c>
+      <c r="G35" s="11">
+        <v>-1980</v>
+      </c>
+      <c r="H35" s="12">
+        <v>-2245</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="30">
+        <v>1</v>
+      </c>
+      <c r="L35" s="31"/>
+      <c r="M35" s="32"/>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>32</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="9">
+        <v>-760</v>
+      </c>
+      <c r="G36" s="11">
+        <v>-606</v>
+      </c>
+      <c r="H36" s="12">
+        <v>-1368</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="30"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>33</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="21">
+        <v>0</v>
+      </c>
+      <c r="D37" s="21">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22">
+        <v>0</v>
+      </c>
+      <c r="F37" s="13">
+        <v>685</v>
+      </c>
+      <c r="G37" s="15">
+        <v>-304</v>
+      </c>
+      <c r="H37" s="16">
+        <v>909</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="33"/>
+      <c r="L37" s="34">
+        <v>1</v>
+      </c>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1">
+        <f>SUM(C5:C37)</f>
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" ref="D38:E38" si="1">SUM(D5:D37)</f>
+        <v>17</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f>SUMPRODUCT(C5:E37,K5:M37)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <f>SUMPRODUCT(C5:C37,F5:F37)</f>
+        <v>178</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B45" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="23">
+        <f>SUMPRODUCT(F5:F37,D5:D37)</f>
+        <v>23463</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B46" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <f>SUMPRODUCT(E5:E37,F5:F37)</f>
+        <v>52756</v>
+      </c>
+      <c r="D46" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47">
+        <f>SUM(D12,D31)</f>
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48">
+        <f>C33+2*D33+3*E33</f>
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48">
+        <f>C35+2*D35+3*E35</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A54861-8CF3-E54E-B295-2CB561EFC1F7}">
+  <dimension ref="A1:M58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>42941</v>
+      </c>
+      <c r="G5" s="7">
+        <v>43411</v>
+      </c>
+      <c r="H5" s="8">
+        <v>11336</v>
+      </c>
+      <c r="I5" s="1">
+        <f>SUM(C5:E5)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="27">
+        <v>1</v>
+      </c>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-917</v>
+      </c>
+      <c r="G6" s="11">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12">
+        <v>-716</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I37" si="0">SUM(C6:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="30"/>
+      <c r="L6" s="31">
+        <v>1</v>
+      </c>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>-6650</v>
+      </c>
+      <c r="G7" s="11">
+        <v>-6244</v>
+      </c>
+      <c r="H7" s="12">
+        <v>-6436</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31">
+        <v>1</v>
+      </c>
+      <c r="M7" s="32"/>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>4</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1941</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1449</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1025</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="30"/>
+      <c r="L8" s="31">
+        <v>1</v>
+      </c>
+      <c r="M8" s="32"/>
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>116</v>
+      </c>
+      <c r="G9" s="11">
+        <v>-871</v>
+      </c>
+      <c r="H9" s="12">
+        <v>-1099</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="30"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>-5194</v>
+      </c>
+      <c r="G10" s="11">
+        <v>-4241</v>
+      </c>
+      <c r="H10" s="12">
+        <v>-5093</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>-299</v>
+      </c>
+      <c r="G11" s="11">
+        <v>223</v>
+      </c>
+      <c r="H11" s="12">
+        <v>567</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31">
+        <v>1</v>
+      </c>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>9790</v>
+      </c>
+      <c r="G12" s="11">
+        <v>8856</v>
+      </c>
+      <c r="H12" s="12">
+        <v>8251</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31">
+        <v>1</v>
+      </c>
+      <c r="M12" s="32"/>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>-6436</v>
+      </c>
+      <c r="G13" s="11">
+        <v>-6787</v>
+      </c>
+      <c r="H13" s="12">
+        <v>-6736</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="30"/>
+      <c r="L13" s="31">
+        <v>1</v>
+      </c>
+      <c r="M13" s="32"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1723</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1993</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1121</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="30"/>
+      <c r="L14" s="31">
+        <v>1</v>
+      </c>
+      <c r="M14" s="32"/>
+    </row>
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>870</v>
+      </c>
+      <c r="G15" s="11">
+        <v>260</v>
+      </c>
+      <c r="H15" s="12">
+        <v>183</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31">
+        <v>1</v>
+      </c>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>12</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>-66</v>
+      </c>
+      <c r="G16" s="11">
+        <v>-349</v>
+      </c>
+      <c r="H16" s="12">
+        <v>-286</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>13</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9">
+        <v>99</v>
+      </c>
+      <c r="G17" s="11">
+        <v>510</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1014</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="30"/>
+      <c r="L17" s="31">
+        <v>1</v>
+      </c>
+      <c r="M17" s="32"/>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>14</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>-8412</v>
+      </c>
+      <c r="G18" s="11">
+        <v>-7585</v>
+      </c>
+      <c r="H18" s="12">
+        <v>-8062</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="30"/>
+      <c r="L18" s="31">
+        <v>1</v>
+      </c>
+      <c r="M18" s="32"/>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>15</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>-3009</v>
+      </c>
+      <c r="G19" s="11">
+        <v>-2233</v>
+      </c>
+      <c r="H19" s="12">
+        <v>-1678</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K19" s="30"/>
+      <c r="L19" s="31">
+        <v>1</v>
+      </c>
+      <c r="M19" s="32"/>
+    </row>
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>395</v>
+      </c>
+      <c r="G20" s="11">
+        <v>-347</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1984</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>17</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>-81</v>
+      </c>
+      <c r="G21" s="11">
+        <v>233</v>
+      </c>
+      <c r="H21" s="12">
+        <v>-371</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="30"/>
+      <c r="L21" s="31">
+        <v>1</v>
+      </c>
+      <c r="M21" s="32"/>
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>18</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>9943</v>
+      </c>
+      <c r="G22" s="11">
+        <v>9995</v>
+      </c>
+      <c r="H22" s="12">
+        <v>9711</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="30"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>19</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1361</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1780</v>
+      </c>
+      <c r="H23" s="12">
+        <v>975</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="30"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>20</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>-5504</v>
+      </c>
+      <c r="G24" s="11">
+        <v>-5578</v>
+      </c>
+      <c r="H24" s="12">
+        <v>-5135</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="30"/>
+      <c r="L24" s="31">
+        <v>1</v>
+      </c>
+      <c r="M24" s="32"/>
+    </row>
+    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>21</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>-812</v>
+      </c>
+      <c r="G25" s="11">
+        <v>-992</v>
+      </c>
+      <c r="H25" s="12">
+        <v>-942</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="30"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>22</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>8016</v>
+      </c>
+      <c r="G26" s="11">
+        <v>7948</v>
+      </c>
+      <c r="H26" s="12">
+        <v>44329</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K26" s="30"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>23</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="9">
+        <v>-2313</v>
+      </c>
+      <c r="G27" s="11">
+        <v>-2665</v>
+      </c>
+      <c r="H27" s="12">
+        <v>-2263</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K27" s="30"/>
+      <c r="L27" s="31">
+        <v>1</v>
+      </c>
+      <c r="M27" s="32"/>
+    </row>
+    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>24</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>2707</v>
+      </c>
+      <c r="G28" s="11">
+        <v>1984</v>
+      </c>
+      <c r="H28" s="12">
+        <v>5668</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>25</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>-13091</v>
+      </c>
+      <c r="G29" s="11">
+        <v>-13942</v>
+      </c>
+      <c r="H29" s="12">
+        <v>-13488</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="30"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>26</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9">
+        <v>6473</v>
+      </c>
+      <c r="G30" s="11">
+        <v>7008</v>
+      </c>
+      <c r="H30" s="12">
+        <v>7571</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="30"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>27</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="9">
+        <v>34523</v>
+      </c>
+      <c r="G31" s="11">
+        <v>34516</v>
+      </c>
+      <c r="H31" s="12">
+        <v>12145</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="30"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>28</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9">
+        <v>-965</v>
+      </c>
+      <c r="G32" s="11">
+        <v>-658</v>
+      </c>
+      <c r="H32" s="12">
+        <v>-173</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="30"/>
+      <c r="L32" s="31">
+        <v>1</v>
+      </c>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>29</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1285</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1491</v>
+      </c>
+      <c r="H33" s="12">
+        <v>3004</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K33" s="30"/>
+      <c r="L33" s="31">
+        <v>1</v>
+      </c>
+      <c r="M33" s="32"/>
+    </row>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>30</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="9">
+        <v>9145</v>
+      </c>
+      <c r="G34" s="11">
+        <v>9779</v>
+      </c>
+      <c r="H34" s="12">
+        <v>10226</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K34" s="30"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>31</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>-1107</v>
+      </c>
+      <c r="G35" s="11">
+        <v>-1980</v>
+      </c>
+      <c r="H35" s="12">
+        <v>-2245</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="30">
+        <v>1</v>
+      </c>
+      <c r="L35" s="31"/>
+      <c r="M35" s="32"/>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>32</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="9">
+        <v>-760</v>
+      </c>
+      <c r="G36" s="11">
+        <v>-606</v>
+      </c>
+      <c r="H36" s="12">
+        <v>-1368</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="30"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>33</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="21">
+        <v>0</v>
+      </c>
+      <c r="D37" s="21">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22">
+        <v>0</v>
+      </c>
+      <c r="F37" s="13">
+        <v>685</v>
+      </c>
+      <c r="G37" s="15">
+        <v>-304</v>
+      </c>
+      <c r="H37" s="16">
+        <v>909</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="33"/>
+      <c r="L37" s="34">
+        <v>1</v>
+      </c>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1">
+        <f>SUM(C5:C37)</f>
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" ref="D38:E38" si="1">SUM(D5:D37)</f>
+        <v>17</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f>SUMPRODUCT(C5:E37,K5:M37)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44">
+        <f>SUMPRODUCT(C5:C37,F5:F37)</f>
+        <v>43119</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B45" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45">
+        <f>SUMPRODUCT(D5:D37,F5:F37)</f>
+        <v>13271</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B46" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46">
+        <f>SUMPRODUCT(E5:E37,F5:F37)</f>
+        <v>20007</v>
+      </c>
+      <c r="D46" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <f>SUMPRODUCT(C5:C37,G5:G37)</f>
+        <v>42922</v>
+      </c>
+      <c r="D47" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="23">
+        <f>SUMPRODUCT(D5:D37,G5:G37)</f>
+        <v>15096</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49">
+        <f>SUMPRODUCT(E5:E37,G5:G37)</f>
+        <v>18054</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B50" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50">
+        <f>SUMPRODUCT(C5:C37,H5:H37)</f>
+        <v>12095</v>
+      </c>
+      <c r="D50" t="s">
+        <v>48</v>
+      </c>
+      <c r="E50">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51">
+        <f>SUMPRODUCT(D5:D37,H5:H37)</f>
+        <v>29723</v>
+      </c>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B52" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52">
+        <f>SUMPRODUCT(E5:E37,H5:H37)</f>
+        <v>22110</v>
+      </c>
+      <c r="D52" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="19"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B56" s="19"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B57" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57">
+        <f>SUM(D12,D31)</f>
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>56</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B58" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58">
+        <f>C33+2*D33+3*E33</f>
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>56</v>
+      </c>
+      <c r="G58">
+        <f>C35+2*D35+3*E35</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>